<commit_message>
Fixed and finished functions
Fixed: addStudents
Finished: changeClassForStudent
</commit_message>
<xml_diff>
--- a/CS162-19APCS2-FinalProjectPlan.xlsx
+++ b/CS162-19APCS2-FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEF354E-404B-41EB-8C39-467AC942B705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDAEE29-1B9E-4650-9985-60BC42F67954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1342,20 +1342,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1858,36 +1858,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
@@ -2017,33 +2017,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
@@ -2222,11 +2222,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2266,26 +2266,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
       <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
@@ -2323,14 +2323,14 @@
       </c>
     </row>
     <row r="3" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -2978,12 +2978,14 @@
       <c r="F16" s="67">
         <v>3</v>
       </c>
-      <c r="G16" s="83">
+      <c r="G16" s="81">
         <v>43960</v>
       </c>
-      <c r="H16" s="67"/>
+      <c r="H16" s="67">
+        <v>4</v>
+      </c>
       <c r="I16" s="68">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J16" s="69"/>
       <c r="K16" s="69"/>
@@ -3019,15 +3021,17 @@
       <c r="E17" s="14">
         <v>11</v>
       </c>
-      <c r="F17" s="85">
+      <c r="F17" s="83">
         <v>3</v>
       </c>
-      <c r="G17" s="84">
+      <c r="G17" s="82">
         <v>43960</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14">
+        <v>4</v>
+      </c>
       <c r="I17" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -3042,10 +3046,10 @@
       <c r="E18" s="14">
         <v>11</v>
       </c>
-      <c r="F18" s="85">
+      <c r="F18" s="83">
         <v>3</v>
       </c>
-      <c r="G18" s="83">
+      <c r="G18" s="81">
         <v>43960</v>
       </c>
       <c r="H18" s="14">
@@ -3067,15 +3071,17 @@
       <c r="E19" s="14">
         <v>11</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="83">
         <v>3</v>
       </c>
-      <c r="G19" s="84">
+      <c r="G19" s="82">
         <v>43960</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="14">
+        <v>4</v>
+      </c>
       <c r="I19" s="15">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -3090,10 +3096,10 @@
       <c r="E20" s="14">
         <v>11</v>
       </c>
-      <c r="F20" s="85">
+      <c r="F20" s="83">
         <v>1</v>
       </c>
-      <c r="G20" s="84">
+      <c r="G20" s="82">
         <v>43962</v>
       </c>
       <c r="H20" s="14">
@@ -3115,10 +3121,10 @@
       <c r="E21" s="14">
         <v>11</v>
       </c>
-      <c r="F21" s="85">
+      <c r="F21" s="83">
         <v>1</v>
       </c>
-      <c r="G21" s="84">
+      <c r="G21" s="82">
         <v>43962</v>
       </c>
       <c r="H21" s="14">

</xml_diff>

<commit_message>
Testing Logging In as student
- Function showMenu throws exception
(break at checking st status)
- Re-updating myself in Plan excel file
</commit_message>
<xml_diff>
--- a/CS162-19APCS2-FinalProjectPlan.xlsx
+++ b/CS162-19APCS2-FinalProjectPlan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9321A6E2-A0AC-4E3D-A50D-8BA0CA472105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53D38BC-278B-4D76-98B5-E5A5B43A456D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -1529,15 +1529,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>16</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>16</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>251460</xdr:rowOff>
+          <xdr:rowOff>254000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1826,16 +1826,16 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="52.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="16.08203125" customWidth="1"/>
+    <col min="3" max="3" width="52.08203125" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="6.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="81" t="s">
         <v>15</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="G1" s="81"/>
       <c r="H1" s="81"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="81"/>
       <c r="B2" s="81"/>
       <c r="C2" s="81"/>
@@ -1857,7 +1857,7 @@
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="81"/>
       <c r="B3" s="81"/>
       <c r="C3" s="81"/>
@@ -1867,7 +1867,7 @@
       <c r="G3" s="81"/>
       <c r="H3" s="81"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>33</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>63</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>16</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
         <v>18</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
         <v>20</v>
       </c>
@@ -1940,7 +1940,7 @@
       <c r="E13" s="27"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
         <v>21</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
         <v>22</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
         <v>23</v>
       </c>
@@ -1985,16 +1985,16 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="27.4140625" customWidth="1"/>
+    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="6" max="6" width="19.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="81" t="s">
         <v>35</v>
       </c>
@@ -2005,7 +2005,7 @@
       <c r="F1" s="81"/>
       <c r="G1" s="81"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="81"/>
       <c r="B2" s="81"/>
       <c r="C2" s="81"/>
@@ -2014,7 +2014,7 @@
       <c r="F2" s="81"/>
       <c r="G2" s="81"/>
     </row>
-    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="81"/>
       <c r="B3" s="81"/>
       <c r="C3" s="81"/>
@@ -2023,7 +2023,7 @@
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
         <v>36</v>
       </c>
@@ -2031,10 +2031,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="17" t="s">
         <v>37</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" s="17"/>
       <c r="C7" t="s">
         <v>126</v>
@@ -2060,7 +2060,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>127</v>
@@ -2069,7 +2069,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="17"/>
       <c r="C9" t="s">
         <v>128</v>
@@ -2078,7 +2078,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
       <c r="C10" t="s">
         <v>124</v>
@@ -2093,14 +2093,14 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="17"/>
       <c r="D11" s="39"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>39</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
@@ -2126,41 +2126,41 @@
       </c>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="17"/>
       <c r="C15" s="29"/>
     </row>
-    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.35">
       <c r="C21" s="59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C22" s="54" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C23" s="54" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C24" s="54" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C25" s="54" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.35">
       <c r="C27" s="63" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.35">
       <c r="C28" s="63" t="s">
         <v>122</v>
       </c>
@@ -2190,51 +2190,51 @@
   </sheetPr>
   <dimension ref="A1:BO81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="T7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="6" topLeftCell="AP25" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="42" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.08203125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="36.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.08203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.08203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="4.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.08203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.77734375" style="1"/>
+    <col min="12" max="12" width="5.08203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.75" style="1"/>
     <col min="14" max="14" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.75" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="1" customWidth="1"/>
     <col min="19" max="19" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="2.77734375" style="1"/>
-    <col min="24" max="24" width="3.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="2.75" style="1"/>
+    <col min="24" max="24" width="3.75" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.6640625" style="1" customWidth="1"/>
-    <col min="26" max="30" width="2.77734375" style="1"/>
+    <col min="26" max="30" width="2.75" style="1"/>
     <col min="31" max="31" width="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.44140625" customWidth="1"/>
-    <col min="38" max="38" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.109375" customWidth="1"/>
-    <col min="45" max="45" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.4140625" customWidth="1"/>
+    <col min="38" max="38" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.08203125" customWidth="1"/>
+    <col min="45" max="45" width="3.75" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B1" s="82" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2246,7 @@
       <c r="H1" s="82"/>
       <c r="I1" s="82"/>
     </row>
-    <row r="2" spans="1:67" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
       <c r="D2" s="82"/>
@@ -2291,7 +2291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
       <c r="D3" s="82"/>
@@ -2306,7 +2306,7 @@
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
     </row>
-    <row r="4" spans="1:67" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:67" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2490,7 +2490,7 @@
       <c r="BN5" s="37"/>
       <c r="BO5" s="38"/>
     </row>
-    <row r="6" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="52" t="s">
         <v>59</v>
@@ -2682,7 +2682,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -2750,7 +2750,7 @@
       <c r="BN7" s="3"/>
       <c r="BO7" s="3"/>
     </row>
-    <row r="8" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>1</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="44">
         <v>1.1000000000000001</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="44">
         <v>1.2</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="44">
         <v>1.3</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="44">
         <v>1.4</v>
       </c>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="44">
         <v>1.5</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43">
         <v>2</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:67" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:67" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="44">
         <v>2.1</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:67" s="61" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:67" s="61" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="64">
         <v>2.2000000000000002</v>
       </c>
@@ -2941,12 +2941,20 @@
       </c>
       <c r="C16" s="66"/>
       <c r="D16" s="74"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
+      <c r="E16" s="67">
+        <v>19</v>
+      </c>
+      <c r="F16" s="67">
+        <v>3</v>
+      </c>
+      <c r="G16" s="67">
+        <v>26</v>
+      </c>
+      <c r="H16" s="67">
+        <v>18</v>
+      </c>
       <c r="I16" s="68">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J16" s="69"/>
       <c r="K16" s="69"/>
@@ -2970,7 +2978,7 @@
       <c r="AC16" s="69"/>
       <c r="AD16" s="69"/>
     </row>
-    <row r="17" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="44">
         <v>2.2999999999999998</v>
       </c>
@@ -2979,13 +2987,23 @@
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="74"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="14">
+        <v>19</v>
+      </c>
+      <c r="F17" s="14">
+        <v>3</v>
+      </c>
+      <c r="G17" s="14">
+        <v>30</v>
+      </c>
+      <c r="H17" s="14">
+        <v>14</v>
+      </c>
+      <c r="I17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="44">
         <v>2.4</v>
       </c>
@@ -2994,13 +3012,23 @@
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="74"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="14">
+        <v>12</v>
+      </c>
+      <c r="F18" s="14">
+        <v>3</v>
+      </c>
+      <c r="G18" s="14">
+        <v>26</v>
+      </c>
+      <c r="H18" s="14">
+        <v>21</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="44">
         <v>2.5</v>
       </c>
@@ -3009,13 +3037,23 @@
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="74"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="14">
+        <v>19</v>
+      </c>
+      <c r="F19" s="14">
+        <v>3</v>
+      </c>
+      <c r="G19" s="14">
+        <v>30</v>
+      </c>
+      <c r="H19" s="14">
+        <v>20</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="44">
         <v>2.6</v>
       </c>
@@ -3024,13 +3062,23 @@
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="74"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="14">
+        <v>12</v>
+      </c>
+      <c r="F20" s="14">
+        <v>3</v>
+      </c>
+      <c r="G20" s="14">
+        <v>26</v>
+      </c>
+      <c r="H20" s="14">
+        <v>7</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="44">
         <v>2.7</v>
       </c>
@@ -3039,13 +3087,23 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="74"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="14">
+        <v>12</v>
+      </c>
+      <c r="F21" s="14">
+        <v>3</v>
+      </c>
+      <c r="G21" s="14">
+        <v>26</v>
+      </c>
+      <c r="H21" s="14">
+        <v>7</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="43">
         <v>3</v>
       </c>
@@ -3061,7 +3119,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="44">
         <v>3.1</v>
       </c>
@@ -3076,7 +3134,7 @@
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="44">
         <v>3.2</v>
       </c>
@@ -3091,7 +3149,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
-    <row r="25" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="44">
         <v>3.3</v>
       </c>
@@ -3106,7 +3164,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
     </row>
-    <row r="26" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="44">
         <v>3.4</v>
       </c>
@@ -3121,7 +3179,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
     </row>
-    <row r="27" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="44">
         <v>3.5</v>
       </c>
@@ -3136,7 +3194,7 @@
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
     </row>
-    <row r="28" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="44">
         <v>3.6</v>
       </c>
@@ -3151,7 +3209,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
     </row>
-    <row r="29" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="44">
         <v>3.7</v>
       </c>
@@ -3166,7 +3224,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
     </row>
-    <row r="30" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="44">
         <v>3.8</v>
       </c>
@@ -3183,7 +3241,7 @@
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="44">
         <v>3.9</v>
       </c>
@@ -3198,7 +3256,7 @@
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="44">
         <v>3.1</v>
       </c>
@@ -3213,7 +3271,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
     </row>
-    <row r="33" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="44">
         <v>3.11</v>
       </c>
@@ -3228,7 +3286,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
     </row>
-    <row r="34" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="43">
         <v>4</v>
       </c>
@@ -3244,7 +3302,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="15"/>
     </row>
-    <row r="35" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="44">
         <v>4.0999999999999996</v>
       </c>
@@ -3259,7 +3317,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="15"/>
     </row>
-    <row r="36" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="44">
         <v>4.2</v>
       </c>
@@ -3274,7 +3332,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="15"/>
     </row>
-    <row r="37" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="43">
         <v>5</v>
       </c>
@@ -3291,7 +3349,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="15"/>
     </row>
-    <row r="38" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="44">
         <v>5.0999999999999996</v>
       </c>
@@ -3306,7 +3364,7 @@
       <c r="H38" s="14"/>
       <c r="I38" s="15"/>
     </row>
-    <row r="39" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="44">
         <v>5.2</v>
       </c>
@@ -3321,7 +3379,7 @@
       <c r="H39" s="14"/>
       <c r="I39" s="15"/>
     </row>
-    <row r="40" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="43">
         <v>6</v>
       </c>
@@ -3337,7 +3395,7 @@
       <c r="H40" s="14"/>
       <c r="I40" s="15"/>
     </row>
-    <row r="41" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="44">
         <v>6.1</v>
       </c>
@@ -3352,7 +3410,7 @@
       <c r="H41" s="14"/>
       <c r="I41" s="15"/>
     </row>
-    <row r="42" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="44">
         <v>6.2</v>
       </c>
@@ -3367,7 +3425,7 @@
       <c r="H42" s="14"/>
       <c r="I42" s="15"/>
     </row>
-    <row r="43" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="44">
         <v>6.3</v>
       </c>
@@ -3382,7 +3440,7 @@
       <c r="H43" s="14"/>
       <c r="I43" s="15"/>
     </row>
-    <row r="44" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="44">
         <v>6.4</v>
       </c>
@@ -3397,7 +3455,7 @@
       <c r="H44" s="14"/>
       <c r="I44" s="15"/>
     </row>
-    <row r="45" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="44">
         <v>6.5</v>
       </c>
@@ -3412,7 +3470,7 @@
       <c r="H45" s="14"/>
       <c r="I45" s="15"/>
     </row>
-    <row r="46" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="44">
         <v>6.6</v>
       </c>
@@ -3427,7 +3485,7 @@
       <c r="H46" s="14"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="44">
         <v>6.7</v>
       </c>
@@ -3442,7 +3500,7 @@
       <c r="H47" s="14"/>
       <c r="I47" s="15"/>
     </row>
-    <row r="48" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="43">
         <v>7</v>
       </c>
@@ -3458,7 +3516,7 @@
       <c r="H48" s="14"/>
       <c r="I48" s="15"/>
     </row>
-    <row r="49" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="44">
         <v>7.1</v>
       </c>
@@ -3473,7 +3531,7 @@
       <c r="H49" s="14"/>
       <c r="I49" s="15"/>
     </row>
-    <row r="50" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="44">
         <v>7.2</v>
       </c>
@@ -3488,7 +3546,7 @@
       <c r="H50" s="14"/>
       <c r="I50" s="15"/>
     </row>
-    <row r="51" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="44">
         <v>7.3</v>
       </c>
@@ -3503,7 +3561,7 @@
       <c r="H51" s="14"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="44">
         <v>7.4</v>
       </c>
@@ -3518,26 +3576,26 @@
       <c r="H52" s="14"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" s="45"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="45"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="45"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B79" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B80" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3596,15 +3654,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>16</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>16</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>251460</xdr:rowOff>
+                    <xdr:rowOff>254000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3633,14 +3691,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="125.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.08203125" customWidth="1"/>
+    <col min="3" max="3" width="125.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>52</v>
       </c>
@@ -3654,7 +3712,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="61" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="61" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="60">
         <v>1.1000000000000001</v>
       </c>
@@ -3664,7 +3722,7 @@
       </c>
       <c r="D3" s="60"/>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="17">
         <v>2.1</v>
       </c>
@@ -3673,12 +3731,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C5" s="55" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="56">
         <v>2.2000000000000002</v>
       </c>
@@ -3686,12 +3744,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C7" s="55" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="56">
         <v>3.2</v>
       </c>
@@ -3699,12 +3757,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C9" s="55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="56">
         <v>3.6</v>
       </c>
@@ -3712,7 +3770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="56">
         <v>3.7</v>
       </c>
@@ -3720,7 +3778,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="56">
         <v>7.1</v>
       </c>
@@ -3728,7 +3786,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="46"/>

</xml_diff>

<commit_message>
fix bugs delete pointer
</commit_message>
<xml_diff>
--- a/CS162-19APCS2-FinalProjectPlan.xlsx
+++ b/CS162-19APCS2-FinalProjectPlan.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9321A6E2-A0AC-4E3D-A50D-8BA0CA472105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -634,7 +633,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -1340,15 +1339,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Activity" xfId="2"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Percent Complete" xfId="6"/>
+    <cellStyle name="Period Headers" xfId="3"/>
+    <cellStyle name="Period Highlight Control" xfId="7"/>
+    <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1578,13 +1577,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
-  <autoFilter ref="C6:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
+  <autoFilter ref="C6:F11"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Github username" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0E6AA203-A562-47F1-A98F-70894F727552}" name="Phone"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="3" name="Email"/>
+    <tableColumn id="4" name="Github username" dataDxfId="10"/>
+    <tableColumn id="2" name="Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1816,7 +1815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1975,7 +1974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -2170,10 +2169,10 @@
     <mergeCell ref="A1:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{3A0AFD0B-1DF5-469B-A887-8713218A0FBE}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{0DC603FB-4850-42AA-AAEE-BBED2A10BF4B}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{A00EE609-315B-4697-A076-F8D226DFA52A}"/>
-    <hyperlink ref="D10" r:id="rId4" xr:uid="{2CBA69B1-0803-42F7-AE93-5C0BEFC5D084}"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2183,7 +2182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2191,11 +2190,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="T7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="T19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -3623,7 +3622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167154E8-4B3C-4AE3-A2D5-CEB0BD01F89A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>

</xml_diff>